<commit_message>
More Analysis Runway exit
</commit_message>
<xml_diff>
--- a/Week 6/Tutorial 5 excel.xlsx
+++ b/Week 6/Tutorial 5 excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barnabas Lim\Downloads\Air-Traffic-Management-master\Air-Traffic-Management-master\Week 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barnabas Lim\Downloads\Air-Traffic-Management-master\Air-Traffic-Management-master\Week 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFA5583-2D8C-4581-9DF1-0A57545FAAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6076F383-3DB1-424D-B232-525767E7A5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E7ADE4EA-C7E9-4B28-88E1-CA509D4986F7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>Flight no</t>
   </si>
@@ -228,12 +228,37 @@
       <t>Discuss the results in question 3 and question 4.</t>
     </r>
   </si>
+  <si>
+    <t>Mean ROT</t>
+  </si>
+  <si>
+    <t>Exit number</t>
+  </si>
+  <si>
+    <t>Exit 1</t>
+  </si>
+  <si>
+    <t>Exit 2</t>
+  </si>
+  <si>
+    <t>Exit 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From question 3, it can be seen that heavier aircraft tends to have a longer ROT than medium craft .
+As a rule of thumb, aircraft typically lands at 1.3 times Stall Speed. This means that a heaveir aircraft will have a higher approach speed(L=W=0.5ρ(V^2)SCl). Assumsing the same braking force, 
+a heavier aircraft will require a longer runway distance and a longer time on runway before exit. This is supported by analysis of the Runway Occupancy Time between Heavy and Medium Aircraft. 
+Heavy Aircraft has a mean ROT of 57.8s while Medium aircraft has a ROT of 50s. 
+It is also important to note that heavy aircraft has a larger standard deviation(7.899s) with ROT values betwee(42s to 73s) while 
+medium aircraft has a smaller standard deviation(4.983s) with ROT values betwee(43s to 57s). This could indicate that there is a larger variance in weight of heavy aircrafts landing
+From questio 4, it can be seen that 
+From question 4, it can be seen that ROT decreases from exit 3,  exit  2 and exit 1. This is expected as runway distance decrease from exit 3, 2, 1. Furthur analysis indicated that very few medium aircraft used exit 2 and none exited from exit 3. Studying the histogram from exit 1. There seems to be two peeks(bimodal shape). This likely indicates that the data comes from two different system. Further analysis shows that one way it can be broken down is by aircraft weight. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +287,14 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -451,11 +484,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -480,6 +681,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -508,11 +715,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,15 +1462,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>414580</xdr:colOff>
+      <xdr:colOff>365344</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>83821</xdr:rowOff>
+      <xdr:rowOff>47679</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1267,8 +1493,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6294121"/>
-          <a:ext cx="3462580" cy="2461260"/>
+          <a:off x="1" y="6388276"/>
+          <a:ext cx="3392466" cy="2490252"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1280,15 +1506,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>525781</xdr:colOff>
+      <xdr:colOff>399200</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>163077</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>464821</xdr:colOff>
+      <xdr:colOff>288255</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>51451</xdr:rowOff>
+      <xdr:rowOff>41754</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1311,8 +1537,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3573781" y="6248400"/>
-          <a:ext cx="3596640" cy="2474611"/>
+          <a:off x="3426323" y="6363461"/>
+          <a:ext cx="3521603" cy="2509142"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1323,16 +1549,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>281836</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>83508</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>110312</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>392148</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>7621</xdr:rowOff>
+      <xdr:rowOff>91128</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1355,8 +1581,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7315200" y="6111241"/>
-          <a:ext cx="3767912" cy="2567940"/>
+          <a:off x="6941507" y="6283892"/>
+          <a:ext cx="3742860" cy="2638085"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1367,23 +1593,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>134230</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>27918</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>496625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>80890</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D74033D-A9C8-48BC-B2D7-91F3965CB178}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83840639-7E89-473B-A51E-BB650B7F78C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1399,56 +1625,17 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11041380" y="6027420"/>
-          <a:ext cx="3810000" cy="2672058"/>
+          <a:off x="7216140" y="3322907"/>
+          <a:ext cx="3643685" cy="2572629"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>344225</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>45721</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83840639-7E89-473B-A51E-BB650B7F78C5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7063740" y="3284221"/>
-          <a:ext cx="3643685" cy="2506980"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1480,7 +1667,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1524,7 +1711,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1533,6 +1720,319 @@
         <a:xfrm>
           <a:off x="0" y="3268981"/>
           <a:ext cx="3513198" cy="2491740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>222369</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>130049</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>2277</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3A1D8DC-0056-4712-B6BD-DF8387FE6773}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11195169" y="6396403"/>
+          <a:ext cx="3811465" cy="2790626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>394138</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>52550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>370895</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>61308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8D3C7DB-4BF9-4B17-A254-83A421DA9A58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9485586" y="1375102"/>
+          <a:ext cx="2429171" cy="1716689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>483127</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>96345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>420414</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F6F3DE7-2CAD-490C-92B8-FFEA5E89F539}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7227265" y="1418897"/>
+          <a:ext cx="2389701" cy="1610326"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>122744</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>142203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581729</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>67652</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE17BED3-F268-441E-AC79-85D5FAAD7CDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="122744" y="14767095"/>
+          <a:ext cx="5912334" cy="3964967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>131379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>313779</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>73068</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C62A032-CAAF-48C2-93D3-3F71EE822E04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9150119"/>
+          <a:ext cx="3340902" cy="2457333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>296234</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>175174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>307235</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>177453</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCD06B58-48D6-4D45-998E-1FFC2AC74D45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3323357" y="9006023"/>
+          <a:ext cx="3643549" cy="2705814"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209368</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>52552</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>481710</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>41753</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91EF0929-E116-42E9-A3D8-F00404BD9288}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6869039" y="9071292"/>
+          <a:ext cx="3904890" cy="2692735"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2948,24 +3448,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D260C8B-AEB5-4C1D-8330-1907975835F5}">
-  <dimension ref="A2:F48"/>
+  <dimension ref="A2:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="U62" sqref="U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="19" width="8.88671875" style="1"/>
+    <col min="20" max="20" width="12.44140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -2974,7 +3477,7 @@
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -2984,7 +3487,7 @@
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
@@ -2994,29 +3497,35 @@
       </c>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="17" t="s">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="5">
         <v>1</v>
       </c>
@@ -3030,8 +3539,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -3054,8 +3563,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
@@ -3076,7 +3585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="6" t="s">
         <v>13</v>
@@ -3098,28 +3607,142 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23" t="s">
+    <row r="17" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+    </row>
+    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R18" s="27"/>
+      <c r="S18" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="T18" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="8"/>
+    </row>
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R19" s="27"/>
+      <c r="S19" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="T19" s="31">
+        <v>57.84</v>
+      </c>
+      <c r="U19" s="8"/>
+    </row>
+    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R20" s="27"/>
+      <c r="S20" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="T20" s="33">
+        <v>50</v>
+      </c>
+      <c r="U20" s="8"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S50" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="T50" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S51" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="T51" s="35">
+        <v>50.53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S52" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="T52" s="31">
+        <v>58.18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S53" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="T53" s="33">
+        <v>67.599999999999994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V60" s="9"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
+    </row>
+    <row r="61" spans="1:25" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
+      <c r="V61" s="26"/>
+      <c r="W61" s="26"/>
+      <c r="X61" s="26"/>
+      <c r="Y61" s="8"/>
+    </row>
+    <row r="62" spans="1:25" ht="155.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="37"/>
+      <c r="O62" s="37"/>
+      <c r="P62" s="37"/>
+      <c r="Q62" s="37"/>
+      <c r="R62" s="37"/>
+      <c r="S62" s="38"/>
+      <c r="V62" s="10"/>
+      <c r="W62" s="10"/>
+      <c r="X62" s="10"/>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="T63" s="24"/>
+      <c r="U63" s="25"/>
+    </row>
+    <row r="71" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A62:S62"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>